<commit_message>
updating terms and making patterns
</commit_message>
<xml_diff>
--- a/terms/femurTerms.xlsx
+++ b/terms/femurTerms.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanabalk/GitHub/futres/fovt/terms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322206FF-EDA4-EA40-9745-5B19407B2D6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C863BD-BEE1-284B-8F66-C35AC3267BFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="3000" windowWidth="26040" windowHeight="14140" activeTab="2" xr2:uid="{CAD560B1-029B-8141-9BD7-72661257BEDC}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16620" activeTab="3" xr2:uid="{CAD560B1-029B-8141-9BD7-72661257BEDC}"/>
   </bookViews>
   <sheets>
     <sheet name="trait" sheetId="1" r:id="rId1"/>
     <sheet name="axis" sheetId="3" r:id="rId2"/>
     <sheet name="AB" sheetId="4" r:id="rId3"/>
-    <sheet name="structures" sheetId="2" r:id="rId4"/>
+    <sheet name="circumferences" sheetId="5" r:id="rId4"/>
+    <sheet name="structures" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="87">
   <si>
     <t>Femur Width Distal 2 (condyles)</t>
   </si>
@@ -241,6 +242,54 @@
   </si>
   <si>
     <t>head of femur</t>
+  </si>
+  <si>
+    <t>Axis</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Pattern name</t>
+  </si>
+  <si>
+    <t>proximal-distal</t>
+  </si>
+  <si>
+    <t>anterior-posterior</t>
+  </si>
+  <si>
+    <t>medial-lateral</t>
+  </si>
+  <si>
+    <t>medial side of' some 'femur'</t>
+  </si>
+  <si>
+    <t>femur medial length</t>
+  </si>
+  <si>
+    <t>diaphysis of femur</t>
+  </si>
+  <si>
+    <t>femur</t>
+  </si>
+  <si>
+    <t>proximal epiphysis of femur</t>
+  </si>
+  <si>
+    <t>distal epiphysis of femur</t>
+  </si>
+  <si>
+    <t>lateral condyle of femur</t>
+  </si>
+  <si>
+    <t>medialmost part of' some 'lesser trochanter'</t>
+  </si>
+  <si>
+    <t>lateralmost part of' some 'greater trochanter'</t>
+  </si>
+  <si>
+    <t>circumference</t>
   </si>
 </sst>
 </file>
@@ -288,12 +337,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,18 +658,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D270C47C-E479-8A43-AE4F-71734E222B7D}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="24.5" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -645,12 +697,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
@@ -661,7 +713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -671,8 +723,14 @@
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
@@ -686,7 +744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -697,7 +755,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -710,8 +768,11 @@
       <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -731,7 +792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -748,7 +809,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -768,7 +829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -791,7 +852,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -805,7 +866,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -825,119 +886,100 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="G14" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="E15" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G15" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="1">
-        <v>8</v>
-      </c>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E24" s="3"/>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="E22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -946,22 +988,159 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BC0F9C-810D-FD4C-B797-65D56A8CDBF1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E96952-7B1C-6B49-A60C-5554849C6390}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1013,12 +1192,60 @@
         <v>line that connects medial condyle of femur and head of femur</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B236827A-831D-C444-B12F-F138F0F72647}">
+  <dimension ref="A2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F6F331-16B8-1B45-AF0E-DBE384939AE3}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>